<commit_message>
Second Commit: Correct version information.
</commit_message>
<xml_diff>
--- a/appInstalls.xlsx
+++ b/appInstalls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Sector108\Npower\Projects\Git\ExcelBasix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{415488AF-E119-433D-992F-3C7FEAB108A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A315B29-0EFF-42CB-AE0C-C169559F2C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="855" windowWidth="29040" windowHeight="16440" xr2:uid="{88250728-926A-45A5-9EA5-88251733CD55}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="33">
   <si>
     <t>install_Id</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>1.1.0</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
   </si>
 </sst>
 </file>
@@ -998,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0A9363-1A55-4C10-8AE4-CD168224C843}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2066,7 +2069,7 @@
         <v>15</v>
       </c>
       <c r="E53" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F53" t="s">
         <v>11</v>

</xml_diff>